<commit_message>
fix package increment issues CI
</commit_message>
<xml_diff>
--- a/src/test/resources/state_counters.xlsx
+++ b/src/test/resources/state_counters.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57901\Downloads\OneMAC-Automation\OneMAC-Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jad92\macpro-onemac-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8A519-5C35-4923-BE47-BF52A390F1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF2AC31-EAF6-4272-AF4D-45786FB3EB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2FB94E9A-B967-4566-B292-1B46864D25D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2FB94E9A-B967-4566-B292-1B46864D25D1}"/>
   </bookViews>
   <sheets>
     <sheet name="StateCounters" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -72,7 +72,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,20 +454,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.85546875"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875"/>
-    <col min="3" max="3" customWidth="true" width="19.28515625"/>
-    <col min="4" max="4" customWidth="true" width="25.42578125"/>
-    <col min="5" max="5" customWidth="true" width="17.140625"/>
-    <col min="6" max="6" customWidth="true" width="36.0"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -488,15 +487,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>9362.0</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>2267.0</v>
+      <c r="B2" s="1">
+        <v>9371</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2267</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -508,15 +507,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>9037.0</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>2230.0</v>
+      <c r="B3" s="1">
+        <v>9037</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2230</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -528,15 +527,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>9031.0</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>2230.0</v>
+      <c r="B4" s="1">
+        <v>9031</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2230</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -548,15 +547,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>9031.0</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2230.0</v>
+      <c r="B5" s="1">
+        <v>9031</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2230</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
testing state counter write back and commit
</commit_message>
<xml_diff>
--- a/src/test/resources/state_counters.xlsx
+++ b/src/test/resources/state_counters.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57901\macpro-onemac-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7806CBA4-EB3A-454C-8671-905ABFD30554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2646524-E2C0-4521-8D37-34889C322825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FB94E9A-B967-4566-B292-1B46864D25D1}"/>
+    <workbookView xWindow="34935" yWindow="1680" windowWidth="21600" windowHeight="11295" xr2:uid="{2FB94E9A-B967-4566-B292-1B46864D25D1}"/>
   </bookViews>
   <sheets>
     <sheet name="StateCounters" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -72,7 +72,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,17 +454,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.85546875"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875"/>
-    <col min="3" max="3" customWidth="true" width="19.28515625"/>
-    <col min="4" max="4" customWidth="true" width="25.42578125"/>
-    <col min="5" max="5" customWidth="true" width="17.140625"/>
-    <col min="6" max="6" customWidth="true" width="36.0"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,11 +491,11 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>9568.0</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>2287.0</v>
+      <c r="B2" s="1">
+        <v>9578</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2287</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>

</xml_diff>